<commit_message>
Implemented gemini llm as part of chatbot
</commit_message>
<xml_diff>
--- a/chatbot-ui/vector-search/rules.xlsx
+++ b/chatbot-ui/vector-search/rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathan\source\repos\AIML\chatbot\chatbot-ui\vector-search\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E581FD74-B6D8-4180-ABF4-479E24554ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F2486C-8A22-47A8-B5D1-AF3B9E38FF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{9035A6CB-C6E4-42A4-B39B-AF854A557D91}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{9035A6CB-C6E4-42A4-B39B-AF854A557D91}"/>
   </bookViews>
   <sheets>
     <sheet name="rules" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>query</t>
   </si>
@@ -29,18 +29,6 @@
     <t>response</t>
   </si>
   <si>
-    <t>How do I reset my password?</t>
-  </si>
-  <si>
-    <t>Click 'Forgot Password' on the login page</t>
-  </si>
-  <si>
-    <t>How do I contact support?</t>
-  </si>
-  <si>
-    <t>Email support@example.com.</t>
-  </si>
-  <si>
     <t>hi</t>
   </si>
   <si>
@@ -81,6 +69,126 @@
   </si>
   <si>
     <t>Goodbye! Have a great day!</t>
+  </si>
+  <si>
+    <t>When can scores be submitted?</t>
+  </si>
+  <si>
+    <t>Scores can be submitted only when all the questions are answered.</t>
+  </si>
+  <si>
+    <t>How are scores 0 and 1 displayed in the report card?</t>
+  </si>
+  <si>
+    <t>Scores 0 and 1 will be displayed in red color in the report card.</t>
+  </si>
+  <si>
+    <t>How is score 2 displayed in the report card?</t>
+  </si>
+  <si>
+    <t>Score 2 will be displayed in orange color in the report card.</t>
+  </si>
+  <si>
+    <t>How is score 3 displayed in the report card?</t>
+  </si>
+  <si>
+    <t>Score 3 will be displayed in green color in the report card.</t>
+  </si>
+  <si>
+    <t>What is the status if no questions are answered in the report card?</t>
+  </si>
+  <si>
+    <t>In a report card, if the questions are not answered, status will be shown as Not Started.</t>
+  </si>
+  <si>
+    <t>What is the status if at least one question is answered in the report card?</t>
+  </si>
+  <si>
+    <t>In a report card, if any one question is answered, status will be shown as In Progress.</t>
+  </si>
+  <si>
+    <t>What is the status if all questions are answered in the report card?</t>
+  </si>
+  <si>
+    <t>In a report card, if all questions are answered, status will be shown as Completed.</t>
+  </si>
+  <si>
+    <t>What happens when all questions are answered regarding percentage?</t>
+  </si>
+  <si>
+    <t>If all the questions are answered, percentage will be shown as 100%.</t>
+  </si>
+  <si>
+    <t>What is the due date for entering scores for the current month?</t>
+  </si>
+  <si>
+    <t>For the current month, due date for entering scores will be the second Friday of the next month.</t>
+  </si>
+  <si>
+    <t>What happens if the score is not submitted before the due date?</t>
+  </si>
+  <si>
+    <t>If the score is not submitted before the due date, the status should be shown as 'Rating Not Complete'.</t>
+  </si>
+  <si>
+    <t>What is the status if the score is submitted before the due date but the due date has passed?</t>
+  </si>
+  <si>
+    <t>If the score is submitted before the due date, then status should be shown as 'Closed' if the due date is crossed.</t>
+  </si>
+  <si>
+    <t>What is the status if the score is submitted before or after the due date?</t>
+  </si>
+  <si>
+    <t>If the score is submitted and the period is before the due date, status will be shown as 'Submitted.' If it is past the due date, then status will be shown as 'Closed.'</t>
+  </si>
+  <si>
+    <t>What happens when 'Score Now' is clicked?</t>
+  </si>
+  <si>
+    <t>On click of 'Score Now', a score dialog will open where we will have 5 questions.</t>
+  </si>
+  <si>
+    <t>What inputs are required when scoring?</t>
+  </si>
+  <si>
+    <t>For each question, we will have to enter a score, and comments are optional.</t>
+  </si>
+  <si>
+    <t>What happens when a score is selected?</t>
+  </si>
+  <si>
+    <t>On selection of scores, corresponding score definitions will be displayed on the right side.</t>
+  </si>
+  <si>
+    <t>When are scores saved?</t>
+  </si>
+  <si>
+    <t>Scores will be saved on selection of the scores.</t>
+  </si>
+  <si>
+    <t>What happens when the reporting period is closed regarding scoring?</t>
+  </si>
+  <si>
+    <t>When Reporting period is closed, scoring should not be enabled.</t>
+  </si>
+  <si>
+    <t>What happens when the reporting period is closed regarding viewing scores?</t>
+  </si>
+  <si>
+    <t>When Reporting period is closed, entered scores can be viewed.</t>
+  </si>
+  <si>
+    <t>What will be displayed to help with scoring in the current month?</t>
+  </si>
+  <si>
+    <t>Previous month scores will be displayed for each question to help score in the current month.</t>
+  </si>
+  <si>
+    <t>How are scores visually represented while entering scores?</t>
+  </si>
+  <si>
+    <t>While entering scores, 0 and 1 shows red color in stepper. 2 shows orange and 3 shows green.</t>
   </si>
 </sst>
 </file>
@@ -921,16 +1029,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1378D724-B063-46B5-8689-9E8522B4FFBC}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="137.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -943,18 +1051,162 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -966,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB7C5E9-D170-441E-AB32-3FD35B6454E0}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -986,58 +1238,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>